<commit_message>
All Projects Push 19Mar21
</commit_message>
<xml_diff>
--- a/Unit-7.6-Capstone-II-DataWrangling/Data/124C_Refinery_MajorCity_Distance.xlsx
+++ b/Unit-7.6-Capstone-II-DataWrangling/Data/124C_Refinery_MajorCity_Distance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\auraimov\Google Drive\SpringBoard\Springboard-DS\Unit-7.6-Capstone-II-DataWrangling\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7AC5CC-A404-44EE-BE2B-DF3CAA8CC9A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898A606D-0AE5-493F-9C88-BC8EC48C2597}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="70" yWindow="0" windowWidth="19490" windowHeight="21600" xr2:uid="{889CBD8A-5E69-4BBB-A83A-EB03B20472E1}"/>
+    <workbookView xWindow="-10" yWindow="10" windowWidth="20860" windowHeight="21600" xr2:uid="{889CBD8A-5E69-4BBB-A83A-EB03B20472E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Distances" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11479" uniqueCount="1473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11479" uniqueCount="1504">
   <si>
     <t>Saraland, Alabama</t>
   </si>
@@ -4453,6 +4453,99 @@
   </si>
   <si>
     <t>1,029 mi</t>
+  </si>
+  <si>
+    <t>534 mi</t>
+  </si>
+  <si>
+    <t>2,084 mi</t>
+  </si>
+  <si>
+    <t>2,082 mi</t>
+  </si>
+  <si>
+    <t>2,200 mi</t>
+  </si>
+  <si>
+    <t>2,072 mi</t>
+  </si>
+  <si>
+    <t>116 mi</t>
+  </si>
+  <si>
+    <t>192 mi</t>
+  </si>
+  <si>
+    <t>652 mi</t>
+  </si>
+  <si>
+    <t>829 mi</t>
+  </si>
+  <si>
+    <t>840 mi</t>
+  </si>
+  <si>
+    <t>873 mi</t>
+  </si>
+  <si>
+    <t>970 mi</t>
+  </si>
+  <si>
+    <t>287 mi</t>
+  </si>
+  <si>
+    <t>713 mi</t>
+  </si>
+  <si>
+    <t>835 mi</t>
+  </si>
+  <si>
+    <t>473 mi</t>
+  </si>
+  <si>
+    <t>985 mi</t>
+  </si>
+  <si>
+    <t>1,077 mi</t>
+  </si>
+  <si>
+    <t>972 mi</t>
+  </si>
+  <si>
+    <t>1,454 mi</t>
+  </si>
+  <si>
+    <t>1,241 mi</t>
+  </si>
+  <si>
+    <t>1,019 mi</t>
+  </si>
+  <si>
+    <t>1,110 mi</t>
+  </si>
+  <si>
+    <t>1,172 mi</t>
+  </si>
+  <si>
+    <t>1,538 mi</t>
+  </si>
+  <si>
+    <t>1,544 mi</t>
+  </si>
+  <si>
+    <t>2,299 mi</t>
+  </si>
+  <si>
+    <t>2,316 mi</t>
+  </si>
+  <si>
+    <t>2,239 mi</t>
+  </si>
+  <si>
+    <t>1,101 mi</t>
+  </si>
+  <si>
+    <t>1,171 mi</t>
   </si>
 </sst>
 </file>
@@ -4949,10 +5042,10 @@
   <dimension ref="A1:JK138"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="AH78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="AI80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AJ91" sqref="AJ91"/>
+      <selection pane="bottomRight" activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -4961,6 +5054,7 @@
     <col min="2" max="3" width="18.36328125" customWidth="1"/>
     <col min="4" max="137" width="18.6328125" customWidth="1"/>
     <col min="138" max="138" width="8.7265625" customWidth="1"/>
+    <col min="139" max="271" width="0" hidden="1" customWidth="1"/>
     <col min="272" max="16384" width="8.7265625" hidden="1"/>
   </cols>
   <sheetData>
@@ -5487,7 +5581,7 @@
         <v>140</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>10</v>
+        <v>735</v>
       </c>
       <c r="AL2" s="4" t="s">
         <v>149</v>
@@ -5800,7 +5894,7 @@
         <v>140</v>
       </c>
       <c r="AK3" s="5" t="s">
-        <v>10</v>
+        <v>1473</v>
       </c>
       <c r="AL3" s="4" t="s">
         <v>149</v>
@@ -7991,7 +8085,7 @@
         <v>140</v>
       </c>
       <c r="AK10" s="5" t="s">
-        <v>10</v>
+        <v>1450</v>
       </c>
       <c r="AL10" s="4" t="s">
         <v>149</v>
@@ -8617,7 +8711,7 @@
         <v>140</v>
       </c>
       <c r="AK12" s="5" t="s">
-        <v>10</v>
+        <v>1454</v>
       </c>
       <c r="AL12" s="4" t="s">
         <v>149</v>
@@ -9869,7 +9963,7 @@
         <v>140</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>10</v>
+        <v>1474</v>
       </c>
       <c r="AL16" s="4" t="s">
         <v>149</v>
@@ -11747,7 +11841,7 @@
         <v>140</v>
       </c>
       <c r="AK22" s="5" t="s">
-        <v>10</v>
+        <v>1475</v>
       </c>
       <c r="AL22" s="4" t="s">
         <v>149</v>
@@ -12060,7 +12154,7 @@
         <v>140</v>
       </c>
       <c r="AK23" s="5" t="s">
-        <v>10</v>
+        <v>1475</v>
       </c>
       <c r="AL23" s="4" t="s">
         <v>149</v>
@@ -12373,7 +12467,7 @@
         <v>140</v>
       </c>
       <c r="AK24" s="5" t="s">
-        <v>10</v>
+        <v>1476</v>
       </c>
       <c r="AL24" s="4" t="s">
         <v>149</v>
@@ -12686,7 +12780,7 @@
         <v>140</v>
       </c>
       <c r="AK25" s="5" t="s">
-        <v>10</v>
+        <v>1477</v>
       </c>
       <c r="AL25" s="4" t="s">
         <v>149</v>
@@ -14564,7 +14658,7 @@
         <v>140</v>
       </c>
       <c r="AK31" s="5" t="s">
-        <v>10</v>
+        <v>1478</v>
       </c>
       <c r="AL31" s="4" t="s">
         <v>149</v>
@@ -15816,7 +15910,7 @@
         <v>140</v>
       </c>
       <c r="AK35" s="5" t="s">
-        <v>10</v>
+        <v>1479</v>
       </c>
       <c r="AL35" s="4" t="s">
         <v>149</v>
@@ -16129,7 +16223,7 @@
         <v>140</v>
       </c>
       <c r="AK36" s="5" t="s">
-        <v>10</v>
+        <v>1480</v>
       </c>
       <c r="AL36" s="4" t="s">
         <v>149</v>
@@ -16442,7 +16536,7 @@
         <v>140</v>
       </c>
       <c r="AK37" s="5" t="s">
-        <v>10</v>
+        <v>315</v>
       </c>
       <c r="AL37" s="4" t="s">
         <v>149</v>
@@ -16755,7 +16849,7 @@
         <v>140</v>
       </c>
       <c r="AK38" s="5" t="s">
-        <v>10</v>
+        <v>821</v>
       </c>
       <c r="AL38" s="4" t="s">
         <v>149</v>
@@ -17068,7 +17162,7 @@
         <v>140</v>
       </c>
       <c r="AK39" s="5" t="s">
-        <v>10</v>
+        <v>1110</v>
       </c>
       <c r="AL39" s="4" t="s">
         <v>149</v>
@@ -17381,7 +17475,7 @@
         <v>140</v>
       </c>
       <c r="AK40" s="5" t="s">
-        <v>1263</v>
+        <v>449</v>
       </c>
       <c r="AL40" s="4" t="s">
         <v>149</v>
@@ -18633,7 +18727,7 @@
         <v>140</v>
       </c>
       <c r="AK44" s="5" t="s">
-        <v>10</v>
+        <v>1481</v>
       </c>
       <c r="AL44" s="4" t="s">
         <v>149</v>
@@ -18946,7 +19040,7 @@
         <v>140</v>
       </c>
       <c r="AK45" s="5" t="s">
-        <v>10</v>
+        <v>1482</v>
       </c>
       <c r="AL45" s="4" t="s">
         <v>149</v>
@@ -19572,7 +19666,7 @@
         <v>140</v>
       </c>
       <c r="AK47" s="5" t="s">
-        <v>1183</v>
+        <v>1483</v>
       </c>
       <c r="AL47" s="4" t="s">
         <v>149</v>
@@ -19885,7 +19979,7 @@
         <v>140</v>
       </c>
       <c r="AK48" s="5" t="s">
-        <v>10</v>
+        <v>1256</v>
       </c>
       <c r="AL48" s="4" t="s">
         <v>149</v>
@@ -20198,7 +20292,7 @@
         <v>140</v>
       </c>
       <c r="AK49" s="5" t="s">
-        <v>10</v>
+        <v>1484</v>
       </c>
       <c r="AL49" s="4" t="s">
         <v>149</v>
@@ -20511,7 +20605,7 @@
         <v>140</v>
       </c>
       <c r="AK50" s="5" t="s">
-        <v>10</v>
+        <v>1256</v>
       </c>
       <c r="AL50" s="4" t="s">
         <v>149</v>
@@ -21763,7 +21857,7 @@
         <v>140</v>
       </c>
       <c r="AK54" s="5" t="s">
-        <v>10</v>
+        <v>740</v>
       </c>
       <c r="AL54" s="4" t="s">
         <v>149</v>
@@ -22389,7 +22483,7 @@
         <v>140</v>
       </c>
       <c r="AK56" s="5" t="s">
-        <v>10</v>
+        <v>1485</v>
       </c>
       <c r="AL56" s="4" t="s">
         <v>149</v>
@@ -23015,7 +23109,7 @@
         <v>140</v>
       </c>
       <c r="AK58" s="5" t="s">
-        <v>10</v>
+        <v>1359</v>
       </c>
       <c r="AL58" s="4" t="s">
         <v>149</v>
@@ -23641,7 +23735,7 @@
         <v>140</v>
       </c>
       <c r="AK60" s="5" t="s">
-        <v>10</v>
+        <v>1486</v>
       </c>
       <c r="AL60" s="4" t="s">
         <v>149</v>
@@ -25206,7 +25300,7 @@
         <v>140</v>
       </c>
       <c r="AK65" s="5" t="s">
-        <v>10</v>
+        <v>1122</v>
       </c>
       <c r="AL65" s="4" t="s">
         <v>149</v>
@@ -25832,7 +25926,7 @@
         <v>140</v>
       </c>
       <c r="AK67" s="5" t="s">
-        <v>10</v>
+        <v>1486</v>
       </c>
       <c r="AL67" s="4" t="s">
         <v>149</v>
@@ -27076,7 +27170,7 @@
         <v>140</v>
       </c>
       <c r="AK71" s="5" t="s">
-        <v>10</v>
+        <v>1357</v>
       </c>
       <c r="AL71" s="4" t="s">
         <v>149</v>
@@ -27387,7 +27481,7 @@
         <v>140</v>
       </c>
       <c r="AK72" s="5" t="s">
-        <v>10</v>
+        <v>1358</v>
       </c>
       <c r="AL72" s="4" t="s">
         <v>149</v>
@@ -28631,7 +28725,7 @@
         <v>140</v>
       </c>
       <c r="AK76" s="5" t="s">
-        <v>10</v>
+        <v>1206</v>
       </c>
       <c r="AL76" s="4" t="s">
         <v>149</v>
@@ -28942,7 +29036,7 @@
         <v>140</v>
       </c>
       <c r="AK77" s="5" t="s">
-        <v>10</v>
+        <v>812</v>
       </c>
       <c r="AL77" s="4" t="s">
         <v>149</v>
@@ -29253,7 +29347,7 @@
         <v>140</v>
       </c>
       <c r="AK78" s="5" t="s">
-        <v>10</v>
+        <v>1487</v>
       </c>
       <c r="AL78" s="4" t="s">
         <v>149</v>
@@ -29564,7 +29658,7 @@
         <v>140</v>
       </c>
       <c r="AK79" s="5" t="s">
-        <v>10</v>
+        <v>1109</v>
       </c>
       <c r="AL79" s="4" t="s">
         <v>149</v>
@@ -30186,7 +30280,7 @@
         <v>140</v>
       </c>
       <c r="AK81" s="5" t="s">
-        <v>10</v>
+        <v>1109</v>
       </c>
       <c r="AL81" s="4" t="s">
         <v>149</v>
@@ -30808,7 +30902,7 @@
         <v>140</v>
       </c>
       <c r="AK83" s="5" t="s">
-        <v>10</v>
+        <v>1480</v>
       </c>
       <c r="AL83" s="4" t="s">
         <v>149</v>
@@ -31119,7 +31213,7 @@
         <v>140</v>
       </c>
       <c r="AK84" s="5" t="s">
-        <v>10</v>
+        <v>1488</v>
       </c>
       <c r="AL84" s="4" t="s">
         <v>149</v>
@@ -32052,7 +32146,7 @@
         <v>140</v>
       </c>
       <c r="AK87" s="5" t="s">
-        <v>10</v>
+        <v>1472</v>
       </c>
       <c r="AL87" s="4" t="s">
         <v>149</v>
@@ -32674,7 +32768,7 @@
         <v>140</v>
       </c>
       <c r="AK89" s="5" t="s">
-        <v>10</v>
+        <v>1472</v>
       </c>
       <c r="AL89" s="4" t="s">
         <v>149</v>
@@ -32985,7 +33079,7 @@
         <v>140</v>
       </c>
       <c r="AK90" s="5" t="s">
-        <v>1472</v>
+        <v>1489</v>
       </c>
       <c r="AL90" s="4" t="s">
         <v>149</v>
@@ -33296,7 +33390,7 @@
         <v>140</v>
       </c>
       <c r="AK91" s="5" t="s">
-        <v>10</v>
+        <v>1472</v>
       </c>
       <c r="AL91" s="4" t="s">
         <v>149</v>
@@ -33607,7 +33701,7 @@
         <v>140</v>
       </c>
       <c r="AK92" s="5" t="s">
-        <v>10</v>
+        <v>209</v>
       </c>
       <c r="AL92" s="4" t="s">
         <v>149</v>
@@ -33918,7 +34012,7 @@
         <v>140</v>
       </c>
       <c r="AK93" s="5" t="s">
-        <v>10</v>
+        <v>513</v>
       </c>
       <c r="AL93" s="4" t="s">
         <v>149</v>
@@ -34229,7 +34323,7 @@
         <v>140</v>
       </c>
       <c r="AK94" s="5" t="s">
-        <v>10</v>
+        <v>513</v>
       </c>
       <c r="AL94" s="4" t="s">
         <v>149</v>
@@ -34540,7 +34634,7 @@
         <v>140</v>
       </c>
       <c r="AK95" s="5" t="s">
-        <v>10</v>
+        <v>1490</v>
       </c>
       <c r="AL95" s="4" t="s">
         <v>149</v>
@@ -34851,7 +34945,7 @@
         <v>140</v>
       </c>
       <c r="AK96" s="5" t="s">
-        <v>10</v>
+        <v>311</v>
       </c>
       <c r="AL96" s="4" t="s">
         <v>149</v>
@@ -35162,7 +35256,7 @@
         <v>140</v>
       </c>
       <c r="AK97" s="5" t="s">
-        <v>10</v>
+        <v>1472</v>
       </c>
       <c r="AL97" s="4" t="s">
         <v>149</v>
@@ -35784,7 +35878,7 @@
         <v>140</v>
       </c>
       <c r="AK99" s="5" t="s">
-        <v>10</v>
+        <v>311</v>
       </c>
       <c r="AL99" s="4" t="s">
         <v>149</v>
@@ -36095,7 +36189,7 @@
         <v>140</v>
       </c>
       <c r="AK100" s="5" t="s">
-        <v>10</v>
+        <v>284</v>
       </c>
       <c r="AL100" s="4" t="s">
         <v>149</v>
@@ -36406,7 +36500,7 @@
         <v>140</v>
       </c>
       <c r="AK101" s="5" t="s">
-        <v>10</v>
+        <v>513</v>
       </c>
       <c r="AL101" s="4" t="s">
         <v>149</v>
@@ -36717,7 +36811,7 @@
         <v>140</v>
       </c>
       <c r="AK102" s="5" t="s">
-        <v>10</v>
+        <v>1491</v>
       </c>
       <c r="AL102" s="4" t="s">
         <v>149</v>
@@ -37028,7 +37122,7 @@
         <v>140</v>
       </c>
       <c r="AK103" s="5" t="s">
-        <v>10</v>
+        <v>1492</v>
       </c>
       <c r="AL103" s="4" t="s">
         <v>149</v>
@@ -37339,7 +37433,7 @@
         <v>140</v>
       </c>
       <c r="AK104" s="5" t="s">
-        <v>10</v>
+        <v>639</v>
       </c>
       <c r="AL104" s="4" t="s">
         <v>149</v>
@@ -37650,7 +37744,7 @@
         <v>140</v>
       </c>
       <c r="AK105" s="5" t="s">
-        <v>10</v>
+        <v>1493</v>
       </c>
       <c r="AL105" s="4" t="s">
         <v>149</v>
@@ -37961,7 +38055,7 @@
         <v>140</v>
       </c>
       <c r="AK106" s="5" t="s">
-        <v>10</v>
+        <v>1494</v>
       </c>
       <c r="AL106" s="4" t="s">
         <v>149</v>
@@ -38272,7 +38366,7 @@
         <v>140</v>
       </c>
       <c r="AK107" s="5" t="s">
-        <v>10</v>
+        <v>1482</v>
       </c>
       <c r="AL107" s="4" t="s">
         <v>149</v>
@@ -38583,7 +38677,7 @@
         <v>140</v>
       </c>
       <c r="AK108" s="5" t="s">
-        <v>10</v>
+        <v>513</v>
       </c>
       <c r="AL108" s="4" t="s">
         <v>149</v>
@@ -38894,7 +38988,7 @@
         <v>140</v>
       </c>
       <c r="AK109" s="5" t="s">
-        <v>10</v>
+        <v>1495</v>
       </c>
       <c r="AL109" s="4" t="s">
         <v>149</v>
@@ -39205,7 +39299,7 @@
         <v>140</v>
       </c>
       <c r="AK110" s="5" t="s">
-        <v>10</v>
+        <v>513</v>
       </c>
       <c r="AL110" s="4" t="s">
         <v>149</v>
@@ -39516,7 +39610,7 @@
         <v>140</v>
       </c>
       <c r="AK111" s="5" t="s">
-        <v>10</v>
+        <v>513</v>
       </c>
       <c r="AL111" s="4" t="s">
         <v>149</v>
@@ -39827,7 +39921,7 @@
         <v>140</v>
       </c>
       <c r="AK112" s="5" t="s">
-        <v>10</v>
+        <v>1494</v>
       </c>
       <c r="AL112" s="4" t="s">
         <v>149</v>
@@ -40138,7 +40232,7 @@
         <v>140</v>
       </c>
       <c r="AK113" s="5" t="s">
-        <v>10</v>
+        <v>311</v>
       </c>
       <c r="AL113" s="4" t="s">
         <v>149</v>
@@ -40449,7 +40543,7 @@
         <v>140</v>
       </c>
       <c r="AK114" s="5" t="s">
-        <v>10</v>
+        <v>1496</v>
       </c>
       <c r="AL114" s="4" t="s">
         <v>149</v>
@@ -40760,7 +40854,7 @@
         <v>140</v>
       </c>
       <c r="AK115" s="5" t="s">
-        <v>10</v>
+        <v>884</v>
       </c>
       <c r="AL115" s="4" t="s">
         <v>149</v>
@@ -41071,7 +41165,7 @@
         <v>140</v>
       </c>
       <c r="AK116" s="5" t="s">
-        <v>10</v>
+        <v>1497</v>
       </c>
       <c r="AL116" s="4" t="s">
         <v>149</v>
@@ -41382,7 +41476,7 @@
         <v>140</v>
       </c>
       <c r="AK117" s="5" t="s">
-        <v>10</v>
+        <v>1498</v>
       </c>
       <c r="AL117" s="4" t="s">
         <v>149</v>
@@ -41693,7 +41787,7 @@
         <v>140</v>
       </c>
       <c r="AK118" s="5" t="s">
-        <v>10</v>
+        <v>549</v>
       </c>
       <c r="AL118" s="4" t="s">
         <v>149</v>
@@ -42004,7 +42098,7 @@
         <v>140</v>
       </c>
       <c r="AK119" s="5" t="s">
-        <v>10</v>
+        <v>1498</v>
       </c>
       <c r="AL119" s="4" t="s">
         <v>149</v>
@@ -42315,7 +42409,7 @@
         <v>140</v>
       </c>
       <c r="AK120" s="5" t="s">
-        <v>10</v>
+        <v>549</v>
       </c>
       <c r="AL120" s="4" t="s">
         <v>149</v>
@@ -42626,7 +42720,7 @@
         <v>140</v>
       </c>
       <c r="AK121" s="5" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="AL121" s="4" t="s">
         <v>149</v>
@@ -42937,7 +43031,7 @@
         <v>140</v>
       </c>
       <c r="AK122" s="5" t="s">
-        <v>10</v>
+        <v>1499</v>
       </c>
       <c r="AL122" s="4" t="s">
         <v>149</v>
@@ -43248,7 +43342,7 @@
         <v>140</v>
       </c>
       <c r="AK123" s="5" t="s">
-        <v>10</v>
+        <v>1499</v>
       </c>
       <c r="AL123" s="4" t="s">
         <v>149</v>
@@ -43559,7 +43653,7 @@
         <v>140</v>
       </c>
       <c r="AK124" s="5" t="s">
-        <v>10</v>
+        <v>1500</v>
       </c>
       <c r="AL124" s="4" t="s">
         <v>149</v>
@@ -43870,7 +43964,7 @@
         <v>140</v>
       </c>
       <c r="AK125" s="5" t="s">
-        <v>10</v>
+        <v>1501</v>
       </c>
       <c r="AL125" s="4" t="s">
         <v>149</v>
@@ -44181,7 +44275,7 @@
         <v>140</v>
       </c>
       <c r="AK126" s="5" t="s">
-        <v>10</v>
+        <v>866</v>
       </c>
       <c r="AL126" s="4" t="s">
         <v>149</v>
@@ -44492,7 +44586,7 @@
         <v>140</v>
       </c>
       <c r="AK127" s="5" t="s">
-        <v>10</v>
+        <v>294</v>
       </c>
       <c r="AL127" s="4" t="s">
         <v>149</v>
@@ -44803,7 +44897,7 @@
         <v>140</v>
       </c>
       <c r="AK128" s="5" t="s">
-        <v>10</v>
+        <v>598</v>
       </c>
       <c r="AL128" s="4" t="s">
         <v>149</v>
@@ -45114,7 +45208,7 @@
         <v>140</v>
       </c>
       <c r="AK129" s="5" t="s">
-        <v>10</v>
+        <v>1502</v>
       </c>
       <c r="AL129" s="4" t="s">
         <v>149</v>
@@ -45425,7 +45519,7 @@
         <v>140</v>
       </c>
       <c r="AK130" s="5" t="s">
-        <v>10</v>
+        <v>532</v>
       </c>
       <c r="AL130" s="4" t="s">
         <v>149</v>
@@ -45736,7 +45830,7 @@
         <v>140</v>
       </c>
       <c r="AK131" s="5" t="s">
-        <v>10</v>
+        <v>1503</v>
       </c>
       <c r="AL131" s="4" t="s">
         <v>149</v>
@@ -46047,7 +46141,7 @@
         <v>140</v>
       </c>
       <c r="AK132" s="7" t="s">
-        <v>10</v>
+        <v>658</v>
       </c>
       <c r="AL132" s="6" t="s">
         <v>149</v>
@@ -46263,455 +46357,455 @@
         <v>10</v>
       </c>
       <c r="G134" s="12">
-        <f t="shared" ref="G134:AL134" si="0">COUNTIF(G$2:G$132,F134)</f>
+        <f t="shared" ref="G134" si="0">COUNTIF(G$2:G$132,F134)</f>
         <v>0</v>
       </c>
       <c r="H134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="I134" s="12">
-        <f t="shared" ref="I134:AN134" si="1">COUNTIF(I$2:I$132,H134)</f>
+        <f t="shared" ref="I134" si="1">COUNTIF(I$2:I$132,H134)</f>
         <v>0</v>
       </c>
       <c r="J134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K134" s="12">
-        <f t="shared" ref="K134:AP134" si="2">COUNTIF(K$2:K$132,J134)</f>
+        <f t="shared" ref="K134" si="2">COUNTIF(K$2:K$132,J134)</f>
         <v>0</v>
       </c>
       <c r="L134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="M134" s="12">
-        <f t="shared" ref="M134:AR134" si="3">COUNTIF(M$2:M$132,L134)</f>
+        <f t="shared" ref="M134" si="3">COUNTIF(M$2:M$132,L134)</f>
         <v>0</v>
       </c>
       <c r="N134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="O134" s="12">
-        <f t="shared" ref="O134:AT134" si="4">COUNTIF(O$2:O$132,N134)</f>
+        <f t="shared" ref="O134" si="4">COUNTIF(O$2:O$132,N134)</f>
         <v>0</v>
       </c>
       <c r="P134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="Q134" s="12">
-        <f t="shared" ref="Q134:AV134" si="5">COUNTIF(Q$2:Q$132,P134)</f>
+        <f t="shared" ref="Q134" si="5">COUNTIF(Q$2:Q$132,P134)</f>
         <v>0</v>
       </c>
       <c r="R134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="S134" s="12">
-        <f t="shared" ref="S134:AX134" si="6">COUNTIF(S$2:S$132,R134)</f>
+        <f t="shared" ref="S134" si="6">COUNTIF(S$2:S$132,R134)</f>
         <v>0</v>
       </c>
       <c r="T134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="U134" s="12">
-        <f t="shared" ref="U134:AZ134" si="7">COUNTIF(U$2:U$132,T134)</f>
+        <f t="shared" ref="U134" si="7">COUNTIF(U$2:U$132,T134)</f>
         <v>0</v>
       </c>
       <c r="V134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="W134" s="12">
-        <f t="shared" ref="W134:BB134" si="8">COUNTIF(W$2:W$132,V134)</f>
+        <f t="shared" ref="W134" si="8">COUNTIF(W$2:W$132,V134)</f>
         <v>0</v>
       </c>
       <c r="X134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="Y134" s="12">
-        <f t="shared" ref="Y134:BD134" si="9">COUNTIF(Y$2:Y$132,X134)</f>
+        <f t="shared" ref="Y134" si="9">COUNTIF(Y$2:Y$132,X134)</f>
         <v>0</v>
       </c>
       <c r="Z134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AA134" s="12">
-        <f t="shared" ref="AA134:BF134" si="10">COUNTIF(AA$2:AA$132,Z134)</f>
+        <f t="shared" ref="AA134" si="10">COUNTIF(AA$2:AA$132,Z134)</f>
         <v>0</v>
       </c>
       <c r="AB134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AC134" s="12">
-        <f t="shared" ref="AC134:BH134" si="11">COUNTIF(AC$2:AC$132,AB134)</f>
+        <f t="shared" ref="AC134" si="11">COUNTIF(AC$2:AC$132,AB134)</f>
         <v>0</v>
       </c>
       <c r="AD134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AE134" s="12">
-        <f t="shared" ref="AE134:BJ134" si="12">COUNTIF(AE$2:AE$132,AD134)</f>
+        <f t="shared" ref="AE134" si="12">COUNTIF(AE$2:AE$132,AD134)</f>
         <v>0</v>
       </c>
       <c r="AF134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AG134" s="12">
-        <f t="shared" ref="AG134:BL134" si="13">COUNTIF(AG$2:AG$132,AF134)</f>
+        <f t="shared" ref="AG134" si="13">COUNTIF(AG$2:AG$132,AF134)</f>
         <v>0</v>
       </c>
       <c r="AH134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AI134" s="12">
-        <f t="shared" ref="AI134:BN134" si="14">COUNTIF(AI$2:AI$132,AH134)</f>
+        <f t="shared" ref="AI134" si="14">COUNTIF(AI$2:AI$132,AH134)</f>
         <v>0</v>
       </c>
       <c r="AJ134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AK134" s="12">
-        <f t="shared" ref="AK134:BP134" si="15">COUNTIF(AK$2:AK$132,AJ134)</f>
-        <v>78</v>
+        <f t="shared" ref="AK134" si="15">COUNTIF(AK$2:AK$132,AJ134)</f>
+        <v>0</v>
       </c>
       <c r="AL134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AM134" s="12">
-        <f t="shared" ref="AM134:BR134" si="16">COUNTIF(AM$2:AM$132,AL134)</f>
+        <f t="shared" ref="AM134" si="16">COUNTIF(AM$2:AM$132,AL134)</f>
         <v>0</v>
       </c>
       <c r="AN134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AO134" s="12">
-        <f t="shared" ref="AO134:BT134" si="17">COUNTIF(AO$2:AO$132,AN134)</f>
+        <f t="shared" ref="AO134" si="17">COUNTIF(AO$2:AO$132,AN134)</f>
         <v>0</v>
       </c>
       <c r="AP134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AQ134" s="12">
-        <f t="shared" ref="AQ134:BV134" si="18">COUNTIF(AQ$2:AQ$132,AP134)</f>
+        <f t="shared" ref="AQ134" si="18">COUNTIF(AQ$2:AQ$132,AP134)</f>
         <v>0</v>
       </c>
       <c r="AR134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AS134" s="12">
-        <f t="shared" ref="AS134:BX134" si="19">COUNTIF(AS$2:AS$132,AR134)</f>
+        <f t="shared" ref="AS134" si="19">COUNTIF(AS$2:AS$132,AR134)</f>
         <v>0</v>
       </c>
       <c r="AT134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AU134" s="12">
-        <f t="shared" ref="AU134:BZ134" si="20">COUNTIF(AU$2:AU$132,AT134)</f>
+        <f t="shared" ref="AU134" si="20">COUNTIF(AU$2:AU$132,AT134)</f>
         <v>0</v>
       </c>
       <c r="AV134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AW134" s="12">
-        <f t="shared" ref="AW134:CB134" si="21">COUNTIF(AW$2:AW$132,AV134)</f>
+        <f t="shared" ref="AW134" si="21">COUNTIF(AW$2:AW$132,AV134)</f>
         <v>0</v>
       </c>
       <c r="AX134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AY134" s="12">
-        <f t="shared" ref="AY134:CD134" si="22">COUNTIF(AY$2:AY$132,AX134)</f>
+        <f t="shared" ref="AY134" si="22">COUNTIF(AY$2:AY$132,AX134)</f>
         <v>0</v>
       </c>
       <c r="AZ134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BA134" s="12">
-        <f t="shared" ref="BA134:CF134" si="23">COUNTIF(BA$2:BA$132,AZ134)</f>
+        <f t="shared" ref="BA134" si="23">COUNTIF(BA$2:BA$132,AZ134)</f>
         <v>0</v>
       </c>
       <c r="BB134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BC134" s="12">
-        <f t="shared" ref="BC134:CH134" si="24">COUNTIF(BC$2:BC$132,BB134)</f>
+        <f t="shared" ref="BC134" si="24">COUNTIF(BC$2:BC$132,BB134)</f>
         <v>0</v>
       </c>
       <c r="BD134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BE134" s="12">
-        <f t="shared" ref="BE134:CJ134" si="25">COUNTIF(BE$2:BE$132,BD134)</f>
+        <f t="shared" ref="BE134" si="25">COUNTIF(BE$2:BE$132,BD134)</f>
         <v>0</v>
       </c>
       <c r="BF134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BG134" s="12">
-        <f t="shared" ref="BG134:CL134" si="26">COUNTIF(BG$2:BG$132,BF134)</f>
+        <f t="shared" ref="BG134" si="26">COUNTIF(BG$2:BG$132,BF134)</f>
         <v>0</v>
       </c>
       <c r="BH134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BI134" s="12">
-        <f t="shared" ref="BI134:CN134" si="27">COUNTIF(BI$2:BI$132,BH134)</f>
+        <f t="shared" ref="BI134" si="27">COUNTIF(BI$2:BI$132,BH134)</f>
         <v>0</v>
       </c>
       <c r="BJ134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BK134" s="12">
-        <f t="shared" ref="BK134:CP134" si="28">COUNTIF(BK$2:BK$132,BJ134)</f>
+        <f t="shared" ref="BK134" si="28">COUNTIF(BK$2:BK$132,BJ134)</f>
         <v>0</v>
       </c>
       <c r="BL134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BM134" s="12">
-        <f t="shared" ref="BM134:CR134" si="29">COUNTIF(BM$2:BM$132,BL134)</f>
+        <f t="shared" ref="BM134" si="29">COUNTIF(BM$2:BM$132,BL134)</f>
         <v>0</v>
       </c>
       <c r="BN134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BO134" s="12">
-        <f t="shared" ref="BO134:CT134" si="30">COUNTIF(BO$2:BO$132,BN134)</f>
+        <f t="shared" ref="BO134" si="30">COUNTIF(BO$2:BO$132,BN134)</f>
         <v>0</v>
       </c>
       <c r="BP134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BQ134" s="12">
-        <f t="shared" ref="BQ134:CV134" si="31">COUNTIF(BQ$2:BQ$132,BP134)</f>
+        <f t="shared" ref="BQ134" si="31">COUNTIF(BQ$2:BQ$132,BP134)</f>
         <v>0</v>
       </c>
       <c r="BR134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BS134" s="12">
-        <f t="shared" ref="BS134:CX134" si="32">COUNTIF(BS$2:BS$132,BR134)</f>
+        <f t="shared" ref="BS134" si="32">COUNTIF(BS$2:BS$132,BR134)</f>
         <v>0</v>
       </c>
       <c r="BT134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BU134" s="12">
-        <f t="shared" ref="BU134:CZ134" si="33">COUNTIF(BU$2:BU$132,BT134)</f>
+        <f t="shared" ref="BU134" si="33">COUNTIF(BU$2:BU$132,BT134)</f>
         <v>0</v>
       </c>
       <c r="BV134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BW134" s="12">
-        <f t="shared" ref="BW134:DB134" si="34">COUNTIF(BW$2:BW$132,BV134)</f>
+        <f t="shared" ref="BW134" si="34">COUNTIF(BW$2:BW$132,BV134)</f>
         <v>0</v>
       </c>
       <c r="BX134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="BY134" s="12">
-        <f t="shared" ref="BY134:DD134" si="35">COUNTIF(BY$2:BY$132,BX134)</f>
+        <f t="shared" ref="BY134" si="35">COUNTIF(BY$2:BY$132,BX134)</f>
         <v>0</v>
       </c>
       <c r="BZ134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CA134" s="12">
-        <f t="shared" ref="CA134:DF134" si="36">COUNTIF(CA$2:CA$132,BZ134)</f>
+        <f t="shared" ref="CA134" si="36">COUNTIF(CA$2:CA$132,BZ134)</f>
         <v>0</v>
       </c>
       <c r="CB134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CC134" s="12">
-        <f t="shared" ref="CC134:DH134" si="37">COUNTIF(CC$2:CC$132,CB134)</f>
+        <f t="shared" ref="CC134" si="37">COUNTIF(CC$2:CC$132,CB134)</f>
         <v>0</v>
       </c>
       <c r="CD134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CE134" s="12">
-        <f t="shared" ref="CE134:DJ134" si="38">COUNTIF(CE$2:CE$132,CD134)</f>
+        <f t="shared" ref="CE134" si="38">COUNTIF(CE$2:CE$132,CD134)</f>
         <v>0</v>
       </c>
       <c r="CF134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CG134" s="12">
-        <f t="shared" ref="CG134:DL134" si="39">COUNTIF(CG$2:CG$132,CF134)</f>
+        <f t="shared" ref="CG134" si="39">COUNTIF(CG$2:CG$132,CF134)</f>
         <v>0</v>
       </c>
       <c r="CH134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CI134" s="12">
-        <f t="shared" ref="CI134:DN134" si="40">COUNTIF(CI$2:CI$132,CH134)</f>
+        <f t="shared" ref="CI134" si="40">COUNTIF(CI$2:CI$132,CH134)</f>
         <v>0</v>
       </c>
       <c r="CJ134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CK134" s="12">
-        <f t="shared" ref="CK134:DP134" si="41">COUNTIF(CK$2:CK$132,CJ134)</f>
+        <f t="shared" ref="CK134" si="41">COUNTIF(CK$2:CK$132,CJ134)</f>
         <v>0</v>
       </c>
       <c r="CL134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CM134" s="12">
-        <f t="shared" ref="CM134:EG134" si="42">COUNTIF(CM$2:CM$132,CL134)</f>
+        <f t="shared" ref="CM134" si="42">COUNTIF(CM$2:CM$132,CL134)</f>
         <v>0</v>
       </c>
       <c r="CN134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CO134" s="12">
-        <f t="shared" ref="CO134:EG134" si="43">COUNTIF(CO$2:CO$132,CN134)</f>
+        <f t="shared" ref="CO134" si="43">COUNTIF(CO$2:CO$132,CN134)</f>
         <v>0</v>
       </c>
       <c r="CP134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CQ134" s="12">
-        <f t="shared" ref="CQ134:EG134" si="44">COUNTIF(CQ$2:CQ$132,CP134)</f>
+        <f t="shared" ref="CQ134" si="44">COUNTIF(CQ$2:CQ$132,CP134)</f>
         <v>0</v>
       </c>
       <c r="CR134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CS134" s="12">
-        <f t="shared" ref="CS134:EG134" si="45">COUNTIF(CS$2:CS$132,CR134)</f>
+        <f t="shared" ref="CS134" si="45">COUNTIF(CS$2:CS$132,CR134)</f>
         <v>0</v>
       </c>
       <c r="CT134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CU134" s="12">
-        <f t="shared" ref="CU134:EG134" si="46">COUNTIF(CU$2:CU$132,CT134)</f>
+        <f t="shared" ref="CU134" si="46">COUNTIF(CU$2:CU$132,CT134)</f>
         <v>0</v>
       </c>
       <c r="CV134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CW134" s="12">
-        <f t="shared" ref="CW134:EG134" si="47">COUNTIF(CW$2:CW$132,CV134)</f>
+        <f t="shared" ref="CW134" si="47">COUNTIF(CW$2:CW$132,CV134)</f>
         <v>0</v>
       </c>
       <c r="CX134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="CY134" s="12">
-        <f t="shared" ref="CY134:EG134" si="48">COUNTIF(CY$2:CY$132,CX134)</f>
+        <f t="shared" ref="CY134" si="48">COUNTIF(CY$2:CY$132,CX134)</f>
         <v>0</v>
       </c>
       <c r="CZ134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DA134" s="12">
-        <f t="shared" ref="DA134:EG134" si="49">COUNTIF(DA$2:DA$132,CZ134)</f>
+        <f t="shared" ref="DA134" si="49">COUNTIF(DA$2:DA$132,CZ134)</f>
         <v>0</v>
       </c>
       <c r="DB134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DC134" s="12">
-        <f t="shared" ref="DC134:EG134" si="50">COUNTIF(DC$2:DC$132,DB134)</f>
+        <f t="shared" ref="DC134" si="50">COUNTIF(DC$2:DC$132,DB134)</f>
         <v>0</v>
       </c>
       <c r="DD134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DE134" s="12">
-        <f t="shared" ref="DE134:EG134" si="51">COUNTIF(DE$2:DE$132,DD134)</f>
+        <f t="shared" ref="DE134" si="51">COUNTIF(DE$2:DE$132,DD134)</f>
         <v>0</v>
       </c>
       <c r="DF134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DG134" s="12">
-        <f t="shared" ref="DG134:EG134" si="52">COUNTIF(DG$2:DG$132,DF134)</f>
+        <f t="shared" ref="DG134" si="52">COUNTIF(DG$2:DG$132,DF134)</f>
         <v>0</v>
       </c>
       <c r="DH134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DI134" s="12">
-        <f t="shared" ref="DI134:EG134" si="53">COUNTIF(DI$2:DI$132,DH134)</f>
+        <f t="shared" ref="DI134" si="53">COUNTIF(DI$2:DI$132,DH134)</f>
         <v>0</v>
       </c>
       <c r="DJ134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DK134" s="12">
-        <f t="shared" ref="DK134:EG134" si="54">COUNTIF(DK$2:DK$132,DJ134)</f>
+        <f t="shared" ref="DK134" si="54">COUNTIF(DK$2:DK$132,DJ134)</f>
         <v>0</v>
       </c>
       <c r="DL134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DM134" s="12">
-        <f t="shared" ref="DM134:EG134" si="55">COUNTIF(DM$2:DM$132,DL134)</f>
+        <f t="shared" ref="DM134" si="55">COUNTIF(DM$2:DM$132,DL134)</f>
         <v>0</v>
       </c>
       <c r="DN134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DO134" s="12">
-        <f t="shared" ref="DO134:EG134" si="56">COUNTIF(DO$2:DO$132,DN134)</f>
+        <f t="shared" ref="DO134" si="56">COUNTIF(DO$2:DO$132,DN134)</f>
         <v>0</v>
       </c>
       <c r="DP134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DQ134" s="12">
-        <f t="shared" ref="DQ134:EG134" si="57">COUNTIF(DQ$2:DQ$132,DP134)</f>
+        <f t="shared" ref="DQ134" si="57">COUNTIF(DQ$2:DQ$132,DP134)</f>
         <v>0</v>
       </c>
       <c r="DR134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DS134" s="12">
-        <f t="shared" ref="DS134:EG134" si="58">COUNTIF(DS$2:DS$132,DR134)</f>
+        <f t="shared" ref="DS134" si="58">COUNTIF(DS$2:DS$132,DR134)</f>
         <v>0</v>
       </c>
       <c r="DT134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DU134" s="12">
-        <f t="shared" ref="DU134:EG134" si="59">COUNTIF(DU$2:DU$132,DT134)</f>
+        <f t="shared" ref="DU134" si="59">COUNTIF(DU$2:DU$132,DT134)</f>
         <v>0</v>
       </c>
       <c r="DV134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DW134" s="12">
-        <f t="shared" ref="DW134:EG134" si="60">COUNTIF(DW$2:DW$132,DV134)</f>
+        <f t="shared" ref="DW134" si="60">COUNTIF(DW$2:DW$132,DV134)</f>
         <v>0</v>
       </c>
       <c r="DX134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="DY134" s="12">
-        <f t="shared" ref="DY134:EG134" si="61">COUNTIF(DY$2:DY$132,DX134)</f>
+        <f t="shared" ref="DY134" si="61">COUNTIF(DY$2:DY$132,DX134)</f>
         <v>0</v>
       </c>
       <c r="DZ134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="EA134" s="12">
-        <f t="shared" ref="EA134:EG134" si="62">COUNTIF(EA$2:EA$132,DZ134)</f>
+        <f t="shared" ref="EA134" si="62">COUNTIF(EA$2:EA$132,DZ134)</f>
         <v>0</v>
       </c>
       <c r="EB134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="EC134" s="12">
-        <f t="shared" ref="EC134:EG134" si="63">COUNTIF(EC$2:EC$132,EB134)</f>
+        <f t="shared" ref="EC134" si="63">COUNTIF(EC$2:EC$132,EB134)</f>
         <v>0</v>
       </c>
       <c r="ED134" s="5" t="s">
         <v>10</v>
       </c>
       <c r="EE134" s="12">
-        <f t="shared" ref="EE134:EG134" si="64">COUNTIF(EE$2:EE$132,ED134)</f>
+        <f t="shared" ref="EE134" si="64">COUNTIF(EE$2:EE$132,ED134)</f>
         <v>0</v>
       </c>
       <c r="EF134" s="5" t="s">

</xml_diff>